<commit_message>
moving to Windows, need to get this stupid visdom server going
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I2"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,51 +442,19 @@
           <t>epoch200</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>epoch250</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>epoch300</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>epoch350</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>epoch400</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>50</v>
+        <v>79.55729141831398</v>
       </c>
       <c r="C2" t="n">
-        <v>50</v>
+        <v>79.55729141831398</v>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>79.55729141831398</v>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G2" t="n">
-        <v>50</v>
-      </c>
-      <c r="H2" t="n">
-        <v>50</v>
-      </c>
-      <c r="I2" t="n">
-        <v>50</v>
+        <v>79.55729141831398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
letting the 02 experiment run
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:E2"/>
+  <dimension ref="B1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,22 +442,54 @@
           <t>epoch200</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>epoch250</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>epoch300</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>epoch350</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>epoch400</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>79.55729141831398</v>
+        <v>81.11979141831398</v>
       </c>
       <c r="C2" t="n">
-        <v>79.55729141831398</v>
+        <v>81.11979141831398</v>
       </c>
       <c r="D2" t="n">
-        <v>79.55729141831398</v>
+        <v>74.58333298563957</v>
       </c>
       <c r="E2" t="n">
-        <v>79.55729141831398</v>
+        <v>66.71874970197678</v>
+      </c>
+      <c r="F2" t="n">
+        <v>63.59374970197678</v>
+      </c>
+      <c r="G2" t="n">
+        <v>61.24999970197678</v>
+      </c>
+      <c r="H2" t="n">
+        <v>58.51562470197678</v>
+      </c>
+      <c r="I2" t="n">
+        <v>58.51562470197678</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
not enough samples, it would seem
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -465,31 +465,31 @@
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>81.11979141831398</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="C2" t="n">
-        <v>81.11979141831398</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="D2" t="n">
-        <v>74.58333298563957</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="E2" t="n">
-        <v>66.71874970197678</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="F2" t="n">
-        <v>63.59374970197678</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="G2" t="n">
-        <v>61.24999970197678</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="H2" t="n">
-        <v>58.51562470197678</v>
+        <v>87.36702129244804</v>
       </c>
       <c r="I2" t="n">
-        <v>58.51562470197678</v>
+        <v>87.36702129244804</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
a whole lot of testing for you babe
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -465,28 +465,28 @@
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>83.67686197161674</v>
+        <v>83.59375</v>
       </c>
       <c r="C2" t="n">
-        <v>83.67686197161674</v>
+        <v>83.59375</v>
       </c>
       <c r="D2" t="n">
-        <v>83.67686197161674</v>
+        <v>83.59375</v>
       </c>
       <c r="E2" t="n">
-        <v>83.67686197161674</v>
+        <v>66.66666666666667</v>
       </c>
       <c r="F2" t="n">
-        <v>83.67686197161674</v>
+        <v>57.55208333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>83.67686197161674</v>
+        <v>54.42708333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>83.67686197161674</v>
+        <v>53.90625</v>
       </c>
       <c r="I2" t="n">
-        <v>83.67686197161674</v>
+        <v>53.90625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a bunch of 3 frame samples to test
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -465,28 +465,28 @@
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>83.59375</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="C2" t="n">
-        <v>83.59375</v>
+        <v>83.33333333333334</v>
       </c>
       <c r="D2" t="n">
-        <v>83.59375</v>
+        <v>81.77083333333334</v>
       </c>
       <c r="E2" t="n">
-        <v>66.66666666666667</v>
+        <v>59.89583333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>57.55208333333333</v>
+        <v>53.125</v>
       </c>
       <c r="G2" t="n">
-        <v>54.42708333333333</v>
+        <v>52.86458333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>53.90625</v>
+        <v>51.82291666666667</v>
       </c>
       <c r="I2" t="n">
-        <v>53.90625</v>
+        <v>51.30208333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trained HCN01 & HCN02
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -465,31 +465,31 @@
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>83.33333333333334</v>
+        <v>58.77403848701053</v>
       </c>
       <c r="C2" t="n">
-        <v>83.33333333333334</v>
+        <v>46.90170917246077</v>
       </c>
       <c r="D2" t="n">
-        <v>81.77083333333334</v>
+        <v>42.64155957433913</v>
       </c>
       <c r="E2" t="n">
-        <v>59.89583333333333</v>
+        <v>41.43963654836019</v>
       </c>
       <c r="F2" t="n">
-        <v>53.125</v>
+        <v>39.75694444444444</v>
       </c>
       <c r="G2" t="n">
-        <v>52.86458333333333</v>
+        <v>39.48985007074144</v>
       </c>
       <c r="H2" t="n">
-        <v>51.82291666666667</v>
+        <v>39.48985007074144</v>
       </c>
       <c r="I2" t="n">
-        <v>51.30208333333333</v>
+        <v>39.40972222222222</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trained a great model!!!!
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN01/best_accuracy_series.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I2"/>
+  <dimension ref="B1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,36 +457,28 @@
           <t>epoch350</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>epoch400</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>58.77403848701053</v>
+        <v>48.32175903850131</v>
       </c>
       <c r="C2" t="n">
-        <v>46.90170917246077</v>
+        <v>38.83101807700263</v>
       </c>
       <c r="D2" t="n">
-        <v>42.64155957433913</v>
+        <v>34.02777777777778</v>
       </c>
       <c r="E2" t="n">
-        <v>41.43963654836019</v>
+        <v>27.60416666666666</v>
       </c>
       <c r="F2" t="n">
-        <v>39.75694444444444</v>
+        <v>25.92592570516798</v>
       </c>
       <c r="G2" t="n">
-        <v>39.48985007074144</v>
+        <v>25.23148126072354</v>
       </c>
       <c r="H2" t="n">
-        <v>39.48985007074144</v>
-      </c>
-      <c r="I2" t="n">
-        <v>39.40972222222222</v>
+        <v>25.23148126072354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>